<commit_message>
handle different pressure units
</commit_message>
<xml_diff>
--- a/MofDB CSV Spec.xlsx
+++ b/MofDB CSV Spec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n8ta/code/mofdb2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C74AA7E-65E8-EB49-95D7-B1390FF98F68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D25BDBA-4796-2741-98D4-37E3E18FCA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{20B8ED7B-40C2-384A-850C-5CAE2281FF85}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
   <si>
     <t>cif_name</t>
   </si>
@@ -130,219 +130,18 @@
     <t>enum-pressure-units</t>
   </si>
   <si>
-    <t xml:space="preserve">"% Volume Adsorbed           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a.u.                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a.u./g                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ang3(STP)/unit cell          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">atoms/unit cell              </t>
-  </si>
-  <si>
     <t xml:space="preserve">cm3(STP)/cm3                 </t>
   </si>
   <si>
     <t xml:space="preserve">cm3(STP)/g                   </t>
   </si>
   <si>
-    <t xml:space="preserve">cm3(STP)/m2                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm3(STP)/mol                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm3/m2                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">coverage                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fractional Coverage          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fractional Loading           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fractional Occupancy         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">g Adsorbate / 100g Adsorbent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/cm3                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/g                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/l                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/ml                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guest molecules per Cu ion   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg/mol                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kmol/m3                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">m3(STP)/kg                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg/g                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg/m2                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">micromoles/m2                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml(STP)/g                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml/g                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol adsorbed                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/cm3                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/g                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/kg                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/m2                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol gas/mol Ni               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/formula unit             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/g                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/l                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/m2                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/m3                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol/mol                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecules Adsorbed           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules*box^-1             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/8 unit cells       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/cage               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/cavity             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/cm2                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/Cu2 unit           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/formula unit       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/fundamental unit   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/nm2                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/pore               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/Rh2 unit           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/site               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/supercage          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/unit pore          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/unitcell           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules/Zn2                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">null                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Occupancy               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">volume/volume                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">wt%                          </t>
-  </si>
-  <si>
     <t xml:space="preserve">atm                          </t>
   </si>
   <si>
     <t xml:space="preserve">bar                          </t>
   </si>
   <si>
-    <t xml:space="preserve">kPa                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mbar                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmHg                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPa                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pa                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">psi                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATIVE                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torr                         </t>
-  </si>
-  <si>
     <t>ATUOYWHBWRKTHZ-UHFFFAOYSA-N</t>
   </si>
   <si>
@@ -421,27 +220,6 @@
     <t>bulk-composition-1</t>
   </si>
   <si>
-    <t>concentration</t>
-  </si>
-  <si>
-    <t>massfraction</t>
-  </si>
-  <si>
-    <t>massratio</t>
-  </si>
-  <si>
-    <t>molefraction</t>
-  </si>
-  <si>
-    <t>moleratio</t>
-  </si>
-  <si>
-    <t>partialpressure</t>
-  </si>
-  <si>
-    <t>relhumidity</t>
-  </si>
-  <si>
     <t>volumefraction</t>
   </si>
   <si>
@@ -458,13 +236,31 @@
   </si>
   <si>
     <t>10.xxx.22222</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>cm3/cm3</t>
+  </si>
+  <si>
+    <t>mg/g</t>
+  </si>
+  <si>
+    <t>mmol/g</t>
+  </si>
+  <si>
+    <t>mol/kg</t>
+  </si>
+  <si>
+    <t>wt%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -520,6 +316,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -541,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +372,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AC2876-B10A-F64C-8755-9E6AAB5BDA06}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,14 +700,14 @@
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -914,7 +718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -928,18 +732,17 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="8" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -950,16 +753,16 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -969,17 +772,14 @@
       <c r="C5" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G5" t="s">
-        <v>130</v>
-      </c>
       <c r="H5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -989,17 +789,12 @@
       <c r="C6" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G6" t="s">
-        <v>131</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -1009,17 +804,13 @@
       <c r="C7" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G7" t="s">
-        <v>132</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1029,17 +820,13 @@
       <c r="C8" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G8" t="s">
-        <v>133</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -1049,17 +836,13 @@
       <c r="C9" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G9" t="s">
-        <v>134</v>
-      </c>
       <c r="H9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
@@ -1069,17 +852,10 @@
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" s="13"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
@@ -1089,17 +865,11 @@
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="7"/>
+      <c r="J11" s="13"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -1109,14 +879,10 @@
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H12" s="7"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
@@ -1126,14 +892,10 @@
       <c r="C13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="7"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1141,27 +903,23 @@
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
@@ -1171,37 +929,31 @@
       <c r="C16" s="9">
         <v>77</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>46</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
@@ -1211,11 +963,9 @@
         <v>26</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>47</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -1225,325 +975,234 @@
         <v>27</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>48</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H22" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>51</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="C24" s="9">
         <v>1.02</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="C25" s="9">
         <v>12</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="C26">
         <v>0.5</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="H27" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>56</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="C29" s="9">
         <v>14</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="C30" s="9">
         <v>100</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="C31" s="9">
         <v>23.23</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H32" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>63</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H37" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H38" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H39" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H40" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H41" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H42" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H43" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H44" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H45" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H46" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H47" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H48" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H49" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="H49" s="7"/>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H50" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H51" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H52" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H53" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H54" s="7" t="s">
-        <v>82</v>
-      </c>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H55" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H56" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H57" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="H57" s="7"/>
     </row>
     <row r="58" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H58" s="7" t="s">
-        <v>86</v>
-      </c>
+      <c r="H58" s="7"/>
     </row>
     <row r="59" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H59" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="H59" s="7"/>
     </row>
     <row r="60" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H60" s="7" t="s">
-        <v>88</v>
-      </c>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H61" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H62" s="7" t="s">
-        <v>90</v>
-      </c>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H63" s="7" t="s">
-        <v>91</v>
-      </c>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H64" s="7" t="s">
-        <v>92</v>
-      </c>
+      <c r="H64" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1592,7 +1251,7 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -1610,45 +1269,45 @@
         <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>0.55400000000000005</v>
@@ -1666,43 +1325,43 @@
         <v>14.5</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>77</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="Q2" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
         <v>29</v>
       </c>
       <c r="S2" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="U2">
         <v>12.2</v>
@@ -1714,7 +1373,7 @@
         <v>0.75</v>
       </c>
       <c r="X2" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="Y2">
         <v>12.2</v>

</xml_diff>